<commit_message>
grobplanung finalisiert, aufgabenverteilung festgelegt, Ziele pberarbeit, Product Backlog gefüllt
</commit_message>
<xml_diff>
--- a/documents/BA.planing.PSP.xlsx
+++ b/documents/BA.planing.PSP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbedo\iCloudDrive\Uni\WS2020\InnoLab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\burak_y46me01\OneDrive\Desktop\BlockchainAccident\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25D20A8-155C-48CF-9E52-934E70BFF3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2367C43-A3FD-4BF8-93AD-1A4D6CB9FE2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2805" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektstrukturplan (PSP)" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
   <si>
     <t>1.1
 Vorarbeit</t>
@@ -300,22 +300,6 @@
 Programming Smart Contracts on Ethereum</t>
   </si>
   <si>
-    <t>1.54.2
-SQL Database Programming on Blockchain</t>
-  </si>
-  <si>
-    <t>1.4.3
-Web Development</t>
-  </si>
-  <si>
-    <t>1.4.4
-Testen/Fehlersuche</t>
-  </si>
-  <si>
-    <t>1.4.5
-Fehlerbehebung/Debugging</t>
-  </si>
-  <si>
     <t>1.5.1
 Tests durchführen</t>
   </si>
@@ -328,10 +312,6 @@
 Verbesserungsanalyse</t>
   </si>
   <si>
-    <t>1.5.4
-Fehlerbearbeitung</t>
-  </si>
-  <si>
     <t>1.6.1
 Aushändigung des Projekts</t>
   </si>
@@ -377,43 +357,55 @@
 Projektziele und Projektabgrenzung (Haupt-, Optional-, Nicht-Ziele)</t>
   </si>
   <si>
+    <t>1.3.11
+Arbeitspaketspez. &amp; Risikobeurteilung</t>
+  </si>
+  <si>
+    <t>1.3.11</t>
+  </si>
+  <si>
+    <t>Umfeldanalyse</t>
+  </si>
+  <si>
+    <t>1.4.2
+IPFS Node Programming on Blockchain</t>
+  </si>
+  <si>
+    <t>1.4.4
+Fehlerbehebung/Debugging</t>
+  </si>
+  <si>
+    <t>1.4.3
+Web3 Development</t>
+  </si>
+  <si>
     <t>1.3.4
-Umfeldanalyse</t>
-  </si>
-  <si>
-    <t>1.3.5
+Risikoplan erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.3.5
+Umfeldanalyse </t>
+  </si>
+  <si>
+    <t>1.3.6
 Ablauf- und Terminplanung
 (Meilensteine, Sprints)</t>
   </si>
   <si>
-    <t>1.3.6
+    <t>1.3.7
 Ressourcenplanung</t>
   </si>
   <si>
-    <t>1.3.7
+    <t>1.3.8
 Auswahl der Programmiersprache</t>
   </si>
   <si>
-    <t>1.3.8
+    <t>1.3.9
 Auswahl des Frameworks</t>
   </si>
   <si>
-    <t>1.3.9
+    <t>1.3.10
 Projektstrukturplan erstellen</t>
-  </si>
-  <si>
-    <t>1.3.10
-Risikoplan erstellen</t>
-  </si>
-  <si>
-    <t>1.3.11
-Arbeitspaketspez. &amp; Risikobeurteilung</t>
-  </si>
-  <si>
-    <t>1.3.11</t>
-  </si>
-  <si>
-    <t>Umfeldanalyse</t>
   </si>
 </sst>
 </file>
@@ -932,23 +924,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.6640625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="11.5546875" style="1"/>
-    <col min="10" max="10" width="11.5546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="28.7109375" style="1" customWidth="1"/>
+    <col min="7" max="9" width="11.5703125" style="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>70</v>
       </c>
@@ -958,8 +950,8 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -979,7 +971,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -987,19 +979,19 @@
         <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>83</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1007,92 +999,86 @@
         <v>68</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>85</v>
+        <v>105</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>91</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C10" s="5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C13" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C15" s="5" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1112,24 +1098,24 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="5.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="11" t="s">
         <v>79</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1137,7 +1123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1145,7 +1131,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1139,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1147,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1155,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1177,7 +1163,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +1171,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1193,7 +1179,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1201,7 +1187,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>71</v>
       </c>
@@ -1209,7 +1195,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>13</v>
       </c>
@@ -1217,7 +1203,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
         <v>14</v>
@@ -1226,7 +1212,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
         <v>15</v>
@@ -1235,7 +1221,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>16</v>
@@ -1244,16 +1230,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
         <v>18</v>
@@ -1262,61 +1248,61 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>22</v>
       </c>
@@ -1324,7 +1310,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
         <v>19</v>
@@ -1333,7 +1319,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>20</v>
@@ -1342,7 +1328,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
         <v>21</v>
@@ -1351,7 +1337,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="6" t="s">
         <v>64</v>
@@ -1360,7 +1346,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
         <v>65</v>
@@ -1369,7 +1355,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>23</v>
       </c>
@@ -1377,7 +1363,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
         <v>48</v>
@@ -1386,7 +1372,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
         <v>49</v>
@@ -1395,7 +1381,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
         <v>50</v>
@@ -1404,7 +1390,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
         <v>54</v>
@@ -1413,7 +1399,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
         <v>47</v>
       </c>
@@ -1421,7 +1407,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
         <v>56</v>
@@ -1430,7 +1416,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
         <v>57</v>
@@ -1439,7 +1425,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
         <v>58</v>
@@ -1448,7 +1434,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
IPFS PROTOKOLL WURDE HINZUGEFÜGT
</commit_message>
<xml_diff>
--- a/documents/BA.planing.PSP.xlsx
+++ b/documents/BA.planing.PSP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbedo\iCloudDrive\Uni\WS2020\InnoLab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ozanaks\Desktop\blockchain\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D25D20A8-155C-48CF-9E52-934E70BFF3AF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2148BD8-38B0-4D54-B02E-9498EB9CA5F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="2805" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21516" yWindow="1092" windowWidth="21600" windowHeight="11388" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Projektstrukturplan (PSP)" sheetId="1" r:id="rId1"/>
@@ -275,9 +275,6 @@
     <t>Programming Smart Contracts on Ethereum</t>
   </si>
   <si>
-    <t>SQL Database Programming on Blockchain</t>
-  </si>
-  <si>
     <t>Web Development</t>
   </si>
   <si>
@@ -298,10 +295,6 @@
   <si>
     <t>1.4.1
 Programming Smart Contracts on Ethereum</t>
-  </si>
-  <si>
-    <t>1.54.2
-SQL Database Programming on Blockchain</t>
   </si>
   <si>
     <t>1.4.3
@@ -414,6 +407,13 @@
   </si>
   <si>
     <t>Umfeldanalyse</t>
+  </si>
+  <si>
+    <t>1.54.2
+IPFS Programming on Blockchain</t>
+  </si>
+  <si>
+    <t>IPFS Programming on Blockchain</t>
   </si>
 </sst>
 </file>
@@ -933,22 +933,22 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="28.6640625" style="1" customWidth="1"/>
-    <col min="7" max="9" width="11.5546875" style="1"/>
-    <col min="10" max="10" width="11.5546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" style="1" customWidth="1"/>
+    <col min="5" max="6" width="28.7109375" style="1" customWidth="1"/>
+    <col min="7" max="9" width="11.5703125" style="1"/>
+    <col min="10" max="10" width="11.5703125" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="32.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="32.25" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>70</v>
       </c>
@@ -958,8 +958,8 @@
       <c r="E1" s="10"/>
       <c r="F1" s="10"/>
     </row>
-    <row r="3" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:6" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:6" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
@@ -970,16 +970,16 @@
         <v>27</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>24</v>
       </c>
@@ -987,19 +987,19 @@
         <v>26</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>25</v>
       </c>
@@ -1007,92 +1007,92 @@
         <v>68</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>84</v>
+        <v>113</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
+    </row>
+    <row r="12" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
+    <row r="13" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="5" t="s">
+    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="5" t="s">
+    <row r="15" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="5" t="s">
-        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1108,28 +1108,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F40"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="50.5546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="5.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50.5703125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="13"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C5" s="6" t="s">
         <v>6</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
@@ -1161,7 +1161,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
         <v>9</v>
       </c>
@@ -1177,7 +1177,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>12</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>71</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="7" t="s">
         <v>13</v>
       </c>
@@ -1217,7 +1217,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
         <v>14</v>
@@ -1226,7 +1226,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
         <v>15</v>
@@ -1235,7 +1235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
         <v>16</v>
@@ -1244,16 +1244,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="6"/>
       <c r="C18" s="6" t="s">
         <v>18</v>
@@ -1262,61 +1262,61 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="7"/>
       <c r="C19" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D19" s="9" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D20" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D21" s="9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
       <c r="C22" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="6"/>
       <c r="C23" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D23" s="9" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="6"/>
       <c r="C24" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D24" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="7" t="s">
         <v>22</v>
       </c>
@@ -1324,7 +1324,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="6"/>
       <c r="C26" s="6" t="s">
         <v>19</v>
@@ -1333,25 +1333,25 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="6"/>
       <c r="C27" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="6"/>
       <c r="C28" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="6"/>
       <c r="C29" s="6" t="s">
         <v>64</v>
@@ -1360,7 +1360,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="6"/>
       <c r="C30" s="6" t="s">
         <v>65</v>
@@ -1369,7 +1369,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>23</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="6"/>
       <c r="C32" s="6" t="s">
         <v>48</v>
@@ -1386,7 +1386,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="6"/>
       <c r="C33" s="6" t="s">
         <v>49</v>
@@ -1395,7 +1395,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="C34" s="6" t="s">
         <v>50</v>
@@ -1404,7 +1404,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="C35" s="6" t="s">
         <v>54</v>
@@ -1413,7 +1413,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="7" t="s">
         <v>47</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="C37" s="6" t="s">
         <v>56</v>
@@ -1430,7 +1430,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="6"/>
       <c r="C38" s="6" t="s">
         <v>57</v>
@@ -1439,7 +1439,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="6"/>
       <c r="C39" s="6" t="s">
         <v>58</v>
@@ -1448,7 +1448,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="6"/>
       <c r="C40" s="6" t="s">
         <v>59</v>

</xml_diff>